<commit_message>
All tests are passing now, including Raders
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9340" yWindow="1780" windowWidth="22900" windowHeight="17440" tabRatio="206"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16280" windowHeight="20560" tabRatio="206"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +242,24 @@
         <bgColor indexed="53"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF21FFFE"/>
+        <bgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="35"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD666E"/>
+        <bgColor indexed="22"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -255,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -269,11 +287,110 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color indexed="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color indexed="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color indexed="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="34"/>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color indexed="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -767,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV37"/>
+  <dimension ref="A1:IW38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W35" sqref="W35"/>
+      <selection activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -778,111 +895,91 @@
     <col min="1" max="16384" width="3.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:43" ht="12.75" customHeight="1">
+      <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="4"/>
-      <c r="AN1" s="4"/>
-      <c r="AO1" s="4"/>
-      <c r="AP1" s="4"/>
-    </row>
-    <row r="2" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -892,16 +989,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>2</v>
@@ -915,57 +1012,59 @@
       <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE2" s="4"/>
+      <c r="AE2" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
@@ -977,10 +1076,11 @@
       <c r="AN2" s="4"/>
       <c r="AO2" s="4"/>
       <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
     </row>
-    <row r="3" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
+    <row r="3" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A3" s="1">
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -989,19 +1089,19 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="G3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>2</v>
@@ -1022,16 +1122,16 @@
         <v>2</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>3</v>
@@ -1048,7 +1148,7 @@
       <c r="W3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="X3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="Y3" s="3" t="s">
@@ -1057,15 +1157,17 @@
       <c r="Z3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA3" s="4"/>
+      <c r="AA3" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="AB3" s="4"/>
-      <c r="AC3" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="AC3" s="4"/>
       <c r="AD3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE3" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
       <c r="AH3" s="4"/>
@@ -1077,36 +1179,37 @@
       <c r="AN3" s="4"/>
       <c r="AO3" s="4"/>
       <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
     </row>
-    <row r="4" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
+    <row r="4" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A4" s="1">
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="3" t="s">
@@ -1122,16 +1225,16 @@
         <v>2</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>3</v>
@@ -1157,15 +1260,17 @@
       <c r="Z4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="4"/>
+      <c r="AA4" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="AB4" s="4"/>
-      <c r="AC4" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="AC4" s="4"/>
       <c r="AD4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE4" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
       <c r="AH4" s="4"/>
@@ -1177,16 +1282,17 @@
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
       <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
     </row>
-    <row r="5" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>11</v>
+    <row r="5" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A5" s="1">
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
@@ -1195,34 +1301,34 @@
         <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="J5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>1</v>
@@ -1234,22 +1340,22 @@
         <v>1</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y5" s="3" t="s">
         <v>3</v>
@@ -1257,15 +1363,17 @@
       <c r="Z5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA5" s="4"/>
+      <c r="AA5" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="AB5" s="4"/>
-      <c r="AC5" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="AC5" s="4"/>
       <c r="AD5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE5" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
@@ -1277,25 +1385,26 @@
       <c r="AN5" s="4"/>
       <c r="AO5" s="4"/>
       <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
     </row>
-    <row r="6" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>1</v>
+    <row r="6" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>1</v>
@@ -1304,19 +1413,19 @@
         <v>1</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>1</v>
@@ -1345,27 +1454,29 @@
       <c r="V6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="W6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="X6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA6" s="4"/>
+      <c r="AA6" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="AB6" s="4"/>
-      <c r="AC6" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="AC6" s="4"/>
       <c r="AD6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE6" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
       <c r="AH6" s="4"/>
@@ -1377,16 +1488,17 @@
       <c r="AN6" s="4"/>
       <c r="AO6" s="4"/>
       <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
     </row>
-    <row r="7" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
+    <row r="7" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>1</v>
@@ -1406,7 +1518,7 @@
       <c r="I7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
@@ -1436,7 +1548,7 @@
       <c r="S7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="T7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="U7" s="3" t="s">
@@ -1448,24 +1560,26 @@
       <c r="W7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="X7" s="3" t="s">
+      <c r="X7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA7" s="4"/>
+      <c r="AA7" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="AB7" s="4"/>
-      <c r="AC7" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="AC7" s="4"/>
       <c r="AD7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE7" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>
@@ -1477,19 +1591,20 @@
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
     </row>
-    <row r="8" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
+    <row r="8" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A8" s="1">
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1</v>
@@ -1498,28 +1613,28 @@
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>1</v>
@@ -1539,7 +1654,7 @@
       <c r="T8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U8" s="3" t="s">
+      <c r="U8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="V8" s="3" t="s">
@@ -1552,20 +1667,22 @@
         <v>1</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA8" s="4"/>
+      <c r="AA8" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="AB8" s="4"/>
-      <c r="AC8" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="AC8" s="4"/>
       <c r="AD8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE8" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="AE8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
       <c r="AH8" s="4"/>
@@ -1577,57 +1694,58 @@
       <c r="AN8" s="4"/>
       <c r="AO8" s="4"/>
       <c r="AP8" s="4"/>
+      <c r="AQ8" s="4"/>
     </row>
-    <row r="9" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
+    <row r="9" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A9" s="1">
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="J9" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -1651,21 +1769,23 @@
       <c r="X9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Y9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA9" s="4"/>
+      <c r="Y9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="AB9" s="4"/>
-      <c r="AC9" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="AC9" s="4"/>
       <c r="AD9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE9" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
       <c r="AH9" s="4"/>
@@ -1677,13 +1797,14 @@
       <c r="AN9" s="4"/>
       <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
+      <c r="AQ9" s="4"/>
     </row>
-    <row r="10" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
+    <row r="10" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A10" s="1">
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>17</v>
@@ -1692,18 +1813,18 @@
         <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="6" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="3" t="s">
@@ -1730,7 +1851,7 @@
       <c r="Q10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="R10" s="9" t="s">
         <v>1</v>
       </c>
       <c r="S10" s="3" t="s">
@@ -1754,14 +1875,20 @@
       <c r="Y10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Z10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="4"/>
+      <c r="Z10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
-      <c r="AD10" s="4"/>
-      <c r="AE10" s="4"/>
+      <c r="AD10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="AF10" s="4"/>
       <c r="AG10" s="4"/>
       <c r="AH10" s="4"/>
@@ -1773,13 +1900,14 @@
       <c r="AN10" s="4"/>
       <c r="AO10" s="4"/>
       <c r="AP10" s="4"/>
+      <c r="AQ10" s="4"/>
     </row>
-    <row r="11" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
+    <row r="11" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A11" s="1">
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>17</v>
@@ -1797,7 +1925,7 @@
         <v>17</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>1</v>
@@ -1806,28 +1934,28 @@
         <v>1</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="S11" s="3" t="s">
         <v>1</v>
@@ -1844,7 +1972,7 @@
       <c r="W11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="X11" s="12" t="s">
+      <c r="X11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Y11" s="3" t="s">
@@ -1853,7 +1981,9 @@
       <c r="Z11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA11" s="4"/>
+      <c r="AA11" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
       <c r="AD11" s="4"/>
@@ -1869,31 +1999,32 @@
       <c r="AN11" s="4"/>
       <c r="AO11" s="4"/>
       <c r="AP11" s="4"/>
+      <c r="AQ11" s="4"/>
     </row>
-    <row r="12" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
+    <row r="12" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A12" s="1">
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>1</v>
@@ -1902,7 +2033,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>23</v>
@@ -1922,12 +2053,12 @@
       <c r="Q12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="R12" s="3" t="s">
+      <c r="R12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="S12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S12" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="T12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1935,25 +2066,25 @@
         <v>1</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="Y12" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA12" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AB12" s="4"/>
-      <c r="AC12" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
@@ -1967,10 +2098,11 @@
       <c r="AN12" s="4"/>
       <c r="AO12" s="4"/>
       <c r="AP12" s="4"/>
+      <c r="AQ12" s="4"/>
     </row>
-    <row r="13" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>1</v>
+    <row r="13" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A13" s="1">
+        <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>1</v>
@@ -1979,11 +2111,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="F13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1996,11 +2128,11 @@
       <c r="I13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>23</v>
@@ -2024,7 +2156,7 @@
         <v>23</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>1</v>
@@ -2032,8 +2164,8 @@
       <c r="U13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="V13" s="7" t="s">
-        <v>27</v>
+      <c r="V13" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="W13" s="3" t="s">
         <v>15</v>
@@ -2047,12 +2179,14 @@
       <c r="Z13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA13" s="4"/>
+      <c r="AA13" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="AB13" s="4"/>
-      <c r="AC13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
       <c r="AG13" s="4"/>
@@ -2065,23 +2199,24 @@
       <c r="AN13" s="4"/>
       <c r="AO13" s="4"/>
       <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
     </row>
-    <row r="14" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
+    <row r="14" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="F14" s="3" t="s">
         <v>1</v>
       </c>
@@ -2097,8 +2232,8 @@
       <c r="J14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>23</v>
+      <c r="K14" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>23</v>
@@ -2122,7 +2257,7 @@
         <v>23</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="T14" s="3" t="s">
         <v>1</v>
@@ -2130,11 +2265,11 @@
       <c r="U14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="V14" s="7" t="s">
+      <c r="V14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W14" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="W14" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="X14" s="3" t="s">
         <v>15</v>
@@ -2142,13 +2277,17 @@
       <c r="Y14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Z14" s="2" t="s">
+      <c r="Z14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA14" s="4"/>
+      <c r="AA14" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
-      <c r="AD14" s="4"/>
+      <c r="AD14" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
       <c r="AG14" s="4"/>
@@ -2161,10 +2300,11 @@
       <c r="AN14" s="4"/>
       <c r="AO14" s="4"/>
       <c r="AP14" s="4"/>
+      <c r="AQ14" s="4"/>
     </row>
-    <row r="15" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
+    <row r="15" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A15" s="1">
+        <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>1</v>
@@ -2173,28 +2313,28 @@
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="F15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>23</v>
@@ -2211,26 +2351,26 @@
       <c r="P15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q15" s="7" t="s">
-        <v>29</v>
+      <c r="Q15" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="R15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="U15" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="V15" s="7" t="s">
+      <c r="U15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="X15" s="3" t="s">
         <v>15</v>
@@ -2241,7 +2381,9 @@
       <c r="Z15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA15" s="4"/>
+      <c r="AA15" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
@@ -2257,10 +2399,11 @@
       <c r="AN15" s="4"/>
       <c r="AO15" s="4"/>
       <c r="AP15" s="4"/>
+      <c r="AQ15" s="4"/>
     </row>
-    <row r="16" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
+    <row r="16" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A16" s="1">
+        <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>1</v>
@@ -2269,52 +2412,52 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>1</v>
+      <c r="J16" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>1</v>
@@ -2322,11 +2465,11 @@
       <c r="U16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="V16" s="7" t="s">
+      <c r="V16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W16" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="W16" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="X16" s="3" t="s">
         <v>15</v>
@@ -2337,7 +2480,9 @@
       <c r="Z16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA16" s="4"/>
+      <c r="AA16" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
       <c r="AD16" s="4"/>
@@ -2353,10 +2498,11 @@
       <c r="AN16" s="4"/>
       <c r="AO16" s="4"/>
       <c r="AP16" s="4"/>
+      <c r="AQ16" s="4"/>
     </row>
-    <row r="17" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
+    <row r="17" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A17" s="1">
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>1</v>
@@ -2368,24 +2514,24 @@
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="3" t="s">
+      <c r="J17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" s="12" t="s">
         <v>1</v>
       </c>
       <c r="L17" s="3" t="s">
@@ -2406,10 +2552,10 @@
       <c r="Q17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="3" t="s">
+      <c r="R17" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="12" t="s">
         <v>1</v>
       </c>
       <c r="T17" s="3" t="s">
@@ -2419,10 +2565,10 @@
         <v>1</v>
       </c>
       <c r="V17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W17" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="X17" s="3" t="s">
         <v>15</v>
@@ -2433,7 +2579,9 @@
       <c r="Z17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA17" s="4"/>
+      <c r="AA17" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="AB17" s="4"/>
       <c r="AC17" s="4"/>
       <c r="AD17" s="4"/>
@@ -2449,55 +2597,56 @@
       <c r="AN17" s="4"/>
       <c r="AO17" s="4"/>
       <c r="AP17" s="4"/>
+      <c r="AQ17" s="4"/>
     </row>
-    <row r="18" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>31</v>
+    <row r="18" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>1</v>
@@ -2517,19 +2666,21 @@
       <c r="V18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="W18" s="8" t="s">
-        <v>1</v>
+      <c r="W18" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
       <c r="AD18" s="4"/>
@@ -2545,16 +2696,17 @@
       <c r="AN18" s="4"/>
       <c r="AO18" s="4"/>
       <c r="AP18" s="4"/>
+      <c r="AQ18" s="4"/>
     </row>
-    <row r="19" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>9</v>
+    <row r="19" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A19" s="1">
+        <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>9</v>
+      <c r="C19" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>9</v>
@@ -2562,8 +2714,8 @@
       <c r="E19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>9</v>
+      <c r="F19" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>9</v>
@@ -2571,8 +2723,8 @@
       <c r="H19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>9</v>
+      <c r="I19" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>9</v>
@@ -2580,8 +2732,8 @@
       <c r="K19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>9</v>
+      <c r="L19" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>9</v>
@@ -2589,16 +2741,16 @@
       <c r="N19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O19" s="3" t="s">
-        <v>9</v>
+      <c r="O19" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="R19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S19" s="3" t="s">
@@ -2608,15 +2760,15 @@
         <v>1</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="V19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="W19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="X19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X19" s="8" t="s">
         <v>1</v>
       </c>
       <c r="Y19" s="3" t="s">
@@ -2625,11 +2777,10 @@
       <c r="Z19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="4">
-        <f>COUNTA(A14:Z14)</f>
-        <v>26</v>
-      </c>
+      <c r="AA19" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
@@ -2644,10 +2795,11 @@
       <c r="AN19" s="4"/>
       <c r="AO19" s="4"/>
       <c r="AP19" s="4"/>
+      <c r="AQ19" s="4"/>
     </row>
-    <row r="20" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>9</v>
+    <row r="20" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A20" s="1">
+        <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>9</v>
@@ -2695,19 +2847,19 @@
         <v>9</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="S20" s="3" t="s">
+      <c r="S20" s="9" t="s">
         <v>1</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="U20" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="V20" s="3" t="s">
         <v>20</v>
@@ -2715,8 +2867,8 @@
       <c r="W20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X20" s="3" t="s">
-        <v>20</v>
+      <c r="X20" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="Y20" s="3" t="s">
         <v>1</v>
@@ -2724,9 +2876,14 @@
       <c r="Z20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA20" s="4"/>
+      <c r="AA20" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AB20" s="4"/>
-      <c r="AC20" s="4"/>
+      <c r="AC20" s="4">
+        <f>COUNTA(B15:AA15)</f>
+        <v>26</v>
+      </c>
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
@@ -2740,10 +2897,11 @@
       <c r="AN20" s="4"/>
       <c r="AO20" s="4"/>
       <c r="AP20" s="4"/>
+      <c r="AQ20" s="4"/>
     </row>
-    <row r="21" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A21" s="3" t="s">
-        <v>9</v>
+    <row r="21" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A21" s="1">
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>9</v>
@@ -2790,17 +2948,17 @@
       <c r="P21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q21" s="10" t="s">
-        <v>1</v>
+      <c r="Q21" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="U21" s="3" t="s">
         <v>20</v>
@@ -2820,7 +2978,9 @@
       <c r="Z21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA21" s="4"/>
+      <c r="AA21" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
@@ -2836,10 +2996,11 @@
       <c r="AN21" s="4"/>
       <c r="AO21" s="4"/>
       <c r="AP21" s="4"/>
+      <c r="AQ21" s="4"/>
     </row>
-    <row r="22" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>9</v>
+    <row r="22" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A22" s="1">
+        <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>9</v>
@@ -2887,13 +3048,13 @@
         <v>9</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R22" s="10" t="s">
         <v>1</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="T22" s="3" t="s">
         <v>20</v>
@@ -2914,9 +3075,11 @@
         <v>20</v>
       </c>
       <c r="Z22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA22" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="AA22" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
       <c r="AD22" s="4"/>
@@ -2932,13 +3095,14 @@
       <c r="AN22" s="4"/>
       <c r="AO22" s="4"/>
       <c r="AP22" s="4"/>
+      <c r="AQ22" s="4"/>
     </row>
-    <row r="23" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>33</v>
+    <row r="23" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>9</v>
@@ -2946,8 +3110,8 @@
       <c r="D23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>33</v>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>9</v>
@@ -2955,8 +3119,8 @@
       <c r="G23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>33</v>
+      <c r="H23" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>9</v>
@@ -2964,8 +3128,8 @@
       <c r="J23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="7" t="s">
-        <v>33</v>
+      <c r="K23" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>9</v>
@@ -2973,8 +3137,8 @@
       <c r="M23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N23" s="11" t="s">
-        <v>33</v>
+      <c r="N23" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>9</v>
@@ -2983,7 +3147,7 @@
         <v>9</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="R23" s="3" t="s">
         <v>1</v>
@@ -3007,12 +3171,14 @@
         <v>20</v>
       </c>
       <c r="Y23" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="Z23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA23" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="AA23" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
       <c r="AD23" s="4"/>
@@ -3028,58 +3194,59 @@
       <c r="AN23" s="4"/>
       <c r="AO23" s="4"/>
       <c r="AP23" s="4"/>
+      <c r="AQ23" s="4"/>
     </row>
-    <row r="24" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>1</v>
+    <row r="24" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A24" s="1">
+        <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="O24" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="R24" s="3" t="s">
         <v>1</v>
@@ -3100,15 +3267,17 @@
         <v>20</v>
       </c>
       <c r="X24" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="Z24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AA24" s="4"/>
+      <c r="AA24" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="4"/>
@@ -3124,87 +3293,90 @@
       <c r="AN24" s="4"/>
       <c r="AO24" s="4"/>
       <c r="AP24" s="4"/>
+      <c r="AQ24" s="4"/>
     </row>
-    <row r="25" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A25" s="7" t="s">
-        <v>34</v>
+    <row r="25" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A25" s="1">
+        <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>34</v>
+        <v>1</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="U25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="V25" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="X25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y25" s="7" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="Y25" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="Z25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA25" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="AA25" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
       <c r="AD25" s="4"/>
@@ -3220,13 +3392,14 @@
       <c r="AN25" s="4"/>
       <c r="AO25" s="4"/>
       <c r="AP25" s="4"/>
+      <c r="AQ25" s="4"/>
     </row>
-    <row r="26" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>7</v>
+    <row r="26" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>7</v>
@@ -3255,13 +3428,13 @@
       <c r="K26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="3" t="s">
-        <v>7</v>
+      <c r="L26" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N26" s="2" t="s">
+      <c r="N26" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O26" s="3" t="s">
@@ -3297,14 +3470,13 @@
       <c r="Y26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Z26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA26" s="4"/>
-      <c r="AB26" s="4">
-        <f>W34</f>
-        <v>0</v>
-      </c>
+      <c r="Z26" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB26" s="4"/>
       <c r="AC26" s="4"/>
       <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
@@ -3319,37 +3491,95 @@
       <c r="AN26" s="4"/>
       <c r="AO26" s="4"/>
       <c r="AP26" s="4"/>
+      <c r="AQ26" s="4"/>
     </row>
-    <row r="27" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
-      <c r="AA27" s="4"/>
+    <row r="27" spans="1:43" ht="15.5" customHeight="1">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA27" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="AB27" s="4"/>
-      <c r="AC27" s="4"/>
+      <c r="AC27" s="4">
+        <f>X35</f>
+        <v>0</v>
+      </c>
       <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
@@ -3363,9 +3593,9 @@
       <c r="AN27" s="4"/>
       <c r="AO27" s="4"/>
       <c r="AP27" s="4"/>
+      <c r="AQ27" s="4"/>
     </row>
-    <row r="28" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A28" s="4"/>
+    <row r="28" spans="1:43" ht="15.5" customHeight="1">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -3407,9 +3637,9 @@
       <c r="AN28" s="4"/>
       <c r="AO28" s="4"/>
       <c r="AP28" s="4"/>
+      <c r="AQ28" s="4"/>
     </row>
-    <row r="29" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:43" ht="15.5" customHeight="1">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -3451,315 +3681,360 @@
       <c r="AN29" s="4"/>
       <c r="AO29" s="4"/>
       <c r="AP29" s="4"/>
+      <c r="AQ29" s="4"/>
     </row>
-    <row r="30" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:43" ht="15.5" customHeight="1">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
+      <c r="AA30" s="4"/>
+      <c r="AB30" s="4"/>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4"/>
+      <c r="AE30" s="4"/>
+      <c r="AF30" s="4"/>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="4"/>
+      <c r="AI30" s="4"/>
+      <c r="AJ30" s="4"/>
+      <c r="AK30" s="4"/>
+      <c r="AL30" s="4"/>
+      <c r="AM30" s="4"/>
+      <c r="AN30" s="4"/>
+      <c r="AO30" s="4"/>
+      <c r="AP30" s="4"/>
+      <c r="AQ30" s="4"/>
+    </row>
+    <row r="31" spans="1:43" ht="15.5" customHeight="1">
+      <c r="B31" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A31" s="5" t="s">
+    <row r="32" spans="1:43" ht="15.5" customHeight="1">
+      <c r="B32" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:42" ht="15.5" customHeight="1">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="2:257" ht="15.5" customHeight="1">
+      <c r="B33" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="Y32"/>
+      <c r="Z33"/>
     </row>
-    <row r="33" spans="1:256" ht="15.5" customHeight="1">
-      <c r="A33" s="8" t="s">
+    <row r="34" spans="2:257" ht="15.5" customHeight="1">
+      <c r="B34" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Y33"/>
+      <c r="Z34"/>
     </row>
-    <row r="34" spans="1:256" ht="15.5" customHeight="1">
-      <c r="A34" s="10" t="s">
+    <row r="35" spans="2:257" ht="15.5" customHeight="1">
+      <c r="B35" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="Y34"/>
+      <c r="Z35"/>
     </row>
-    <row r="35" spans="1:256" ht="15.5" customHeight="1">
-      <c r="A35" s="6" t="s">
+    <row r="36" spans="2:257" ht="15.5" customHeight="1">
+      <c r="B36" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
-      <c r="AE35"/>
-      <c r="AF35"/>
-      <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
-      <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35"/>
-      <c r="AQ35"/>
-      <c r="AR35"/>
-      <c r="AS35"/>
-      <c r="AT35"/>
-      <c r="AU35"/>
-      <c r="AV35"/>
-      <c r="AW35"/>
-      <c r="AX35"/>
-      <c r="AY35"/>
-      <c r="AZ35"/>
-      <c r="BA35"/>
-      <c r="BB35"/>
-      <c r="BC35"/>
-      <c r="BD35"/>
-      <c r="BE35"/>
-      <c r="BF35"/>
-      <c r="BG35"/>
-      <c r="BH35"/>
-      <c r="BI35"/>
-      <c r="BJ35"/>
-      <c r="BK35"/>
-      <c r="BL35"/>
-      <c r="BM35"/>
-      <c r="BN35"/>
-      <c r="BO35"/>
-      <c r="BP35"/>
-      <c r="BQ35"/>
-      <c r="BR35"/>
-      <c r="BS35"/>
-      <c r="BT35"/>
-      <c r="BU35"/>
-      <c r="BV35"/>
-      <c r="BW35"/>
-      <c r="BX35"/>
-      <c r="BY35"/>
-      <c r="BZ35"/>
-      <c r="CA35"/>
-      <c r="CB35"/>
-      <c r="CC35"/>
-      <c r="CD35"/>
-      <c r="CE35"/>
-      <c r="CF35"/>
-      <c r="CG35"/>
-      <c r="CH35"/>
-      <c r="CI35"/>
-      <c r="CJ35"/>
-      <c r="CK35"/>
-      <c r="CL35"/>
-      <c r="CM35"/>
-      <c r="CN35"/>
-      <c r="CO35"/>
-      <c r="CP35"/>
-      <c r="CQ35"/>
-      <c r="CR35"/>
-      <c r="CS35"/>
-      <c r="CT35"/>
-      <c r="CU35"/>
-      <c r="CV35"/>
-      <c r="CW35"/>
-      <c r="CX35"/>
-      <c r="CY35"/>
-      <c r="CZ35"/>
-      <c r="DA35"/>
-      <c r="DB35"/>
-      <c r="DC35"/>
-      <c r="DD35"/>
-      <c r="DE35"/>
-      <c r="DF35"/>
-      <c r="DG35"/>
-      <c r="DH35"/>
-      <c r="DI35"/>
-      <c r="DJ35"/>
-      <c r="DK35"/>
-      <c r="DL35"/>
-      <c r="DM35"/>
-      <c r="DN35"/>
-      <c r="DO35"/>
-      <c r="DP35"/>
-      <c r="DQ35"/>
-      <c r="DR35"/>
-      <c r="DS35"/>
-      <c r="DT35"/>
-      <c r="DU35"/>
-      <c r="DV35"/>
-      <c r="DW35"/>
-      <c r="DX35"/>
-      <c r="DY35"/>
-      <c r="DZ35"/>
-      <c r="EA35"/>
-      <c r="EB35"/>
-      <c r="EC35"/>
-      <c r="ED35"/>
-      <c r="EE35"/>
-      <c r="EF35"/>
-      <c r="EG35"/>
-      <c r="EH35"/>
-      <c r="EI35"/>
-      <c r="EJ35"/>
-      <c r="EK35"/>
-      <c r="EL35"/>
-      <c r="EM35"/>
-      <c r="EN35"/>
-      <c r="EO35"/>
-      <c r="EP35"/>
-      <c r="EQ35"/>
-      <c r="ER35"/>
-      <c r="ES35"/>
-      <c r="ET35"/>
-      <c r="EU35"/>
-      <c r="EV35"/>
-      <c r="EW35"/>
-      <c r="EX35"/>
-      <c r="EY35"/>
-      <c r="EZ35"/>
-      <c r="FA35"/>
-      <c r="FB35"/>
-      <c r="FC35"/>
-      <c r="FD35"/>
-      <c r="FE35"/>
-      <c r="FF35"/>
-      <c r="FG35"/>
-      <c r="FH35"/>
-      <c r="FI35"/>
-      <c r="FJ35"/>
-      <c r="FK35"/>
-      <c r="FL35"/>
-      <c r="FM35"/>
-      <c r="FN35"/>
-      <c r="FO35"/>
-      <c r="FP35"/>
-      <c r="FQ35"/>
-      <c r="FR35"/>
-      <c r="FS35"/>
-      <c r="FT35"/>
-      <c r="FU35"/>
-      <c r="FV35"/>
-      <c r="FW35"/>
-      <c r="FX35"/>
-      <c r="FY35"/>
-      <c r="FZ35"/>
-      <c r="GA35"/>
-      <c r="GB35"/>
-      <c r="GC35"/>
-      <c r="GD35"/>
-      <c r="GE35"/>
-      <c r="GF35"/>
-      <c r="GG35"/>
-      <c r="GH35"/>
-      <c r="GI35"/>
-      <c r="GJ35"/>
-      <c r="GK35"/>
-      <c r="GL35"/>
-      <c r="GM35"/>
-      <c r="GN35"/>
-      <c r="GO35"/>
-      <c r="GP35"/>
-      <c r="GQ35"/>
-      <c r="GR35"/>
-      <c r="GS35"/>
-      <c r="GT35"/>
-      <c r="GU35"/>
-      <c r="GV35"/>
-      <c r="GW35"/>
-      <c r="GX35"/>
-      <c r="GY35"/>
-      <c r="GZ35"/>
-      <c r="HA35"/>
-      <c r="HB35"/>
-      <c r="HC35"/>
-      <c r="HD35"/>
-      <c r="HE35"/>
-      <c r="HF35"/>
-      <c r="HG35"/>
-      <c r="HH35"/>
-      <c r="HI35"/>
-      <c r="HJ35"/>
-      <c r="HK35"/>
-      <c r="HL35"/>
-      <c r="HM35"/>
-      <c r="HN35"/>
-      <c r="HO35"/>
-      <c r="HP35"/>
-      <c r="HQ35"/>
-      <c r="HR35"/>
-      <c r="HS35"/>
-      <c r="HT35"/>
-      <c r="HU35"/>
-      <c r="HV35"/>
-      <c r="HW35"/>
-      <c r="HX35"/>
-      <c r="HY35"/>
-      <c r="HZ35"/>
-      <c r="IA35"/>
-      <c r="IB35"/>
-      <c r="IC35"/>
-      <c r="ID35"/>
-      <c r="IE35"/>
-      <c r="IF35"/>
-      <c r="IG35"/>
-      <c r="IH35"/>
-      <c r="II35"/>
-      <c r="IJ35"/>
-      <c r="IK35"/>
-      <c r="IL35"/>
-      <c r="IM35"/>
-      <c r="IN35"/>
-      <c r="IO35"/>
-      <c r="IP35"/>
-      <c r="IQ35"/>
-      <c r="IR35"/>
-      <c r="IS35"/>
-      <c r="IT35"/>
-      <c r="IU35"/>
-      <c r="IV35"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AJ36"/>
+      <c r="AK36"/>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+      <c r="AR36"/>
+      <c r="AS36"/>
+      <c r="AT36"/>
+      <c r="AU36"/>
+      <c r="AV36"/>
+      <c r="AW36"/>
+      <c r="AX36"/>
+      <c r="AY36"/>
+      <c r="AZ36"/>
+      <c r="BA36"/>
+      <c r="BB36"/>
+      <c r="BC36"/>
+      <c r="BD36"/>
+      <c r="BE36"/>
+      <c r="BF36"/>
+      <c r="BG36"/>
+      <c r="BH36"/>
+      <c r="BI36"/>
+      <c r="BJ36"/>
+      <c r="BK36"/>
+      <c r="BL36"/>
+      <c r="BM36"/>
+      <c r="BN36"/>
+      <c r="BO36"/>
+      <c r="BP36"/>
+      <c r="BQ36"/>
+      <c r="BR36"/>
+      <c r="BS36"/>
+      <c r="BT36"/>
+      <c r="BU36"/>
+      <c r="BV36"/>
+      <c r="BW36"/>
+      <c r="BX36"/>
+      <c r="BY36"/>
+      <c r="BZ36"/>
+      <c r="CA36"/>
+      <c r="CB36"/>
+      <c r="CC36"/>
+      <c r="CD36"/>
+      <c r="CE36"/>
+      <c r="CF36"/>
+      <c r="CG36"/>
+      <c r="CH36"/>
+      <c r="CI36"/>
+      <c r="CJ36"/>
+      <c r="CK36"/>
+      <c r="CL36"/>
+      <c r="CM36"/>
+      <c r="CN36"/>
+      <c r="CO36"/>
+      <c r="CP36"/>
+      <c r="CQ36"/>
+      <c r="CR36"/>
+      <c r="CS36"/>
+      <c r="CT36"/>
+      <c r="CU36"/>
+      <c r="CV36"/>
+      <c r="CW36"/>
+      <c r="CX36"/>
+      <c r="CY36"/>
+      <c r="CZ36"/>
+      <c r="DA36"/>
+      <c r="DB36"/>
+      <c r="DC36"/>
+      <c r="DD36"/>
+      <c r="DE36"/>
+      <c r="DF36"/>
+      <c r="DG36"/>
+      <c r="DH36"/>
+      <c r="DI36"/>
+      <c r="DJ36"/>
+      <c r="DK36"/>
+      <c r="DL36"/>
+      <c r="DM36"/>
+      <c r="DN36"/>
+      <c r="DO36"/>
+      <c r="DP36"/>
+      <c r="DQ36"/>
+      <c r="DR36"/>
+      <c r="DS36"/>
+      <c r="DT36"/>
+      <c r="DU36"/>
+      <c r="DV36"/>
+      <c r="DW36"/>
+      <c r="DX36"/>
+      <c r="DY36"/>
+      <c r="DZ36"/>
+      <c r="EA36"/>
+      <c r="EB36"/>
+      <c r="EC36"/>
+      <c r="ED36"/>
+      <c r="EE36"/>
+      <c r="EF36"/>
+      <c r="EG36"/>
+      <c r="EH36"/>
+      <c r="EI36"/>
+      <c r="EJ36"/>
+      <c r="EK36"/>
+      <c r="EL36"/>
+      <c r="EM36"/>
+      <c r="EN36"/>
+      <c r="EO36"/>
+      <c r="EP36"/>
+      <c r="EQ36"/>
+      <c r="ER36"/>
+      <c r="ES36"/>
+      <c r="ET36"/>
+      <c r="EU36"/>
+      <c r="EV36"/>
+      <c r="EW36"/>
+      <c r="EX36"/>
+      <c r="EY36"/>
+      <c r="EZ36"/>
+      <c r="FA36"/>
+      <c r="FB36"/>
+      <c r="FC36"/>
+      <c r="FD36"/>
+      <c r="FE36"/>
+      <c r="FF36"/>
+      <c r="FG36"/>
+      <c r="FH36"/>
+      <c r="FI36"/>
+      <c r="FJ36"/>
+      <c r="FK36"/>
+      <c r="FL36"/>
+      <c r="FM36"/>
+      <c r="FN36"/>
+      <c r="FO36"/>
+      <c r="FP36"/>
+      <c r="FQ36"/>
+      <c r="FR36"/>
+      <c r="FS36"/>
+      <c r="FT36"/>
+      <c r="FU36"/>
+      <c r="FV36"/>
+      <c r="FW36"/>
+      <c r="FX36"/>
+      <c r="FY36"/>
+      <c r="FZ36"/>
+      <c r="GA36"/>
+      <c r="GB36"/>
+      <c r="GC36"/>
+      <c r="GD36"/>
+      <c r="GE36"/>
+      <c r="GF36"/>
+      <c r="GG36"/>
+      <c r="GH36"/>
+      <c r="GI36"/>
+      <c r="GJ36"/>
+      <c r="GK36"/>
+      <c r="GL36"/>
+      <c r="GM36"/>
+      <c r="GN36"/>
+      <c r="GO36"/>
+      <c r="GP36"/>
+      <c r="GQ36"/>
+      <c r="GR36"/>
+      <c r="GS36"/>
+      <c r="GT36"/>
+      <c r="GU36"/>
+      <c r="GV36"/>
+      <c r="GW36"/>
+      <c r="GX36"/>
+      <c r="GY36"/>
+      <c r="GZ36"/>
+      <c r="HA36"/>
+      <c r="HB36"/>
+      <c r="HC36"/>
+      <c r="HD36"/>
+      <c r="HE36"/>
+      <c r="HF36"/>
+      <c r="HG36"/>
+      <c r="HH36"/>
+      <c r="HI36"/>
+      <c r="HJ36"/>
+      <c r="HK36"/>
+      <c r="HL36"/>
+      <c r="HM36"/>
+      <c r="HN36"/>
+      <c r="HO36"/>
+      <c r="HP36"/>
+      <c r="HQ36"/>
+      <c r="HR36"/>
+      <c r="HS36"/>
+      <c r="HT36"/>
+      <c r="HU36"/>
+      <c r="HV36"/>
+      <c r="HW36"/>
+      <c r="HX36"/>
+      <c r="HY36"/>
+      <c r="HZ36"/>
+      <c r="IA36"/>
+      <c r="IB36"/>
+      <c r="IC36"/>
+      <c r="ID36"/>
+      <c r="IE36"/>
+      <c r="IF36"/>
+      <c r="IG36"/>
+      <c r="IH36"/>
+      <c r="II36"/>
+      <c r="IJ36"/>
+      <c r="IK36"/>
+      <c r="IL36"/>
+      <c r="IM36"/>
+      <c r="IN36"/>
+      <c r="IO36"/>
+      <c r="IP36"/>
+      <c r="IQ36"/>
+      <c r="IR36"/>
+      <c r="IS36"/>
+      <c r="IT36"/>
+      <c r="IU36"/>
+      <c r="IV36"/>
+      <c r="IW36"/>
     </row>
-    <row r="36" spans="1:256" ht="15.5" customHeight="1">
-      <c r="A36" s="12" t="s">
+    <row r="37" spans="2:257" ht="15.5" customHeight="1">
+      <c r="B37" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Y36"/>
+      <c r="Z37"/>
     </row>
-    <row r="37" spans="1:256" ht="15.5" customHeight="1">
-      <c r="A37" s="11" t="s">
+    <row r="38" spans="2:257" ht="15.5" customHeight="1">
+      <c r="B38" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="Y37"/>
+      <c r="Z38"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <conditionalFormatting sqref="A1:A5 A7:A12 A14:A26 A30 B1:G26 H1:H8 H10:H26 I1:I26 J1:J3 J5:J6 J8:J12 J14:J15 J17:J26 K1:M26 N1:N7 N9:N22 N24:N26 O1:O26 P1:P2 P4:P26 Q1:Q8 Q10:Q20 Q22:Q26 R1:R15 R17:R18 R20:R26 S1:S26 T1:T6 T8:T26 U1:U14 U16:U26 V1:V26 W1 W3:W5 W7:W17 W19:W26 X1:X10 X12:X26 Y1:Y26 Z1:Z17 Z19:Z26">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>NOT(ISERROR(SEARCH("X",A1)))</formula>
+  <conditionalFormatting sqref="B2:B6 B8:B13 B15:B27 B31 C2:H27 I2:I9 I11:I27 J2:J27 K2:K4 K6:K7 K9:K13 K15:K16 K18:K27 L2:N27 O3:O8 O10:O23 O25:O27 P2:P27 Q2:Q3 Q5:Q27 R2:R9 R11:R16 R23:R27 S2:S16 S18:S19 S21:S27 T2:T27 U2:U7 U9:U27 V2:V15 V17:V27 W2:W27 X2 X4:X6 X8:X18 X20:X27 Y2:Y11 Y13:Y27 Z2:Z27 AA2:AA18 AA20:AA27 R18:R21">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+      <formula>NOT(ISERROR(SEARCH("X",B2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>NOT(ISERROR(SEARCH("W",A1)))</formula>
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+      <formula>NOT(ISERROR(SEARCH("W",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>